<commit_message>
Added Listener and Reporting Feature
</commit_message>
<xml_diff>
--- a/Data Source.xlsx
+++ b/Data Source.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\OrangeHRM\OrangeHRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C269D2FD-3F6A-4D8B-9D34-A834C63CF7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F6C4ED-F279-4621-B932-F88203F88006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="8170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="credentials" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>newUserName</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Vishwanath D B</t>
+  </si>
+  <si>
+    <t>iVLq@23JjQ</t>
+  </si>
+  <si>
+    <t>Tabby</t>
+  </si>
+  <si>
+    <t>TabbyUpdate</t>
   </si>
 </sst>
 </file>
@@ -118,13 +127,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,7 +419,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,32 +431,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="mailto:Password@123" xr:uid="{FE1FA66B-AA19-4712-BB82-777CBD5968E4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6EAD0F-7112-47DC-8A85-FF77FB3076E9}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,36 +512,51 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="mailto:Password@123" xr:uid="{4B0E18DB-04E6-4BE6-A1D6-10F806008452}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{E269F121-5E98-4D8D-9DAA-FC5FA725EF16}"/>
+    <hyperlink ref="B4" r:id="rId2" display="mailto:Password@123" xr:uid="{950CE2AA-8BC0-4609-9EC6-29D9E8936F22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Maven TestNG Integration
</commit_message>
<xml_diff>
--- a/Data Source.xlsx
+++ b/Data Source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\OrangeHRM\OrangeHRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F6C4ED-F279-4621-B932-F88203F88006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA2E18B-BF82-4DE9-BB23-EC2ED109AC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="8170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>newUserName</t>
   </si>
@@ -52,32 +52,32 @@
     <t>Aaron Update</t>
   </si>
   <si>
+    <t>iVLq@23JjQ</t>
+  </si>
+  <si>
+    <t>Tabby</t>
+  </si>
+  <si>
+    <t>TabbyUpdate</t>
+  </si>
+  <si>
     <t>Vish</t>
   </si>
   <si>
-    <t>Password@123</t>
-  </si>
-  <si>
-    <t>Vishwanath</t>
-  </si>
-  <si>
-    <t>Vishwanath D B</t>
-  </si>
-  <si>
-    <t>iVLq@23JjQ</t>
-  </si>
-  <si>
-    <t>Tabby</t>
-  </si>
-  <si>
-    <t>TabbyUpdate</t>
+    <t>free@123</t>
+  </si>
+  <si>
+    <t>Fun</t>
+  </si>
+  <si>
+    <t>Joy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,12 +87,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,16 +119,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,35 +450,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="mailto:Password@123" xr:uid="{FE1FA66B-AA19-4712-BB82-777CBD5968E4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6EAD0F-7112-47DC-8A85-FF77FB3076E9}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,48 +490,34 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{E269F121-5E98-4D8D-9DAA-FC5FA725EF16}"/>
-    <hyperlink ref="B4" r:id="rId2" display="mailto:Password@123" xr:uid="{950CE2AA-8BC0-4609-9EC6-29D9E8936F22}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{4E115366-D6D7-4D78-9778-801B289CC976}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>